<commit_message>
Commit Three from VS Code
</commit_message>
<xml_diff>
--- a/mappings/store_mapping.xlsx
+++ b/mappings/store_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\risha\VS CODE PROJECTS\wholefoods-to-xoro\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E533CAAC-1021-44DA-A697-5114FA8BF1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C31056-F907-4CCD-AEDC-0BEA3601B78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FA61781-5299-4C23-8C4C-619A5C9AB8B5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FA61781-5299-4C23-8C4C-619A5C9AB8B5}"/>
   </bookViews>
   <sheets>
     <sheet name="store_mapping" sheetId="1" r:id="rId1"/>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>